<commit_message>
Actualizacion tiempo cada integrante del equipo
</commit_message>
<xml_diff>
--- a/Primera Entrega/Control Asignaciones.xlsx
+++ b/Primera Entrega/Control Asignaciones.xlsx
@@ -5,21 +5,21 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\Desktop\METODOS FORMALES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SEMANA 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="56">
   <si>
     <t>Entrega de todos los documentos finales al líder de soporte</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Fecha Acordada</t>
   </si>
   <si>
-    <t>Para</t>
-  </si>
-  <si>
     <t>De</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
     <t xml:space="preserve">Ciclo: </t>
   </si>
   <si>
-    <t xml:space="preserve">PROYECTO:  </t>
-  </si>
-  <si>
     <t>Universidad Piloto de Colombia</t>
   </si>
   <si>
@@ -175,6 +169,24 @@
   </si>
   <si>
     <t>LS-LD</t>
+  </si>
+  <si>
+    <t>Tiempo Estimado (minutos)</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>Definir objetivos y métricas rol de líder de arquitectura</t>
+  </si>
+  <si>
+    <t>Roles</t>
+  </si>
+  <si>
+    <t>Minutos trabajados por tarea</t>
+  </si>
+  <si>
+    <t>PROYECTO:  RAPICOOP</t>
   </si>
 </sst>
 </file>
@@ -186,7 +198,7 @@
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="166" formatCode="_ [$€-2]\ * #,##0.00_ ;_ [$€-2]\ * \-#,##0.00_ ;_ [$€-2]\ * &quot;-&quot;??_ "/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -236,6 +248,17 @@
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -449,7 +472,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -505,6 +528,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -622,6 +656,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D56D3492-D519-4696-87A0-D7FF07AF2AF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11020425" y="0"/>
+          <a:ext cx="1638300" cy="619125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -946,114 +1030,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="53.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="4" customWidth="1"/>
     <col min="3" max="6" width="10.7109375" style="4" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" style="3" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" style="3" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" style="2" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="48.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" style="1" customWidth="1"/>
     <col min="12" max="12" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="28"/>
-      <c r="B1" s="30" t="s">
+      <c r="A1" s="33"/>
+      <c r="B1" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="38"/>
+    </row>
+    <row r="2" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="34"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="40"/>
+    </row>
+    <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="46"/>
+    </row>
+    <row r="4" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="42"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="33"/>
-    </row>
-    <row r="2" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="35"/>
-    </row>
-    <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" s="41"/>
-    </row>
-    <row r="4" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="24" t="s">
-        <v>13</v>
-      </c>
       <c r="K4" s="23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="27"/>
-    </row>
-    <row r="7" spans="1:11" s="20" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="32"/>
+    </row>
+    <row r="7" spans="1:11" s="20" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="22" t="s">
         <v>9</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>50</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>8</v>
@@ -1082,23 +1166,25 @@
     </row>
     <row r="8" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="26">
+        <v>20</v>
+      </c>
       <c r="D8" s="12">
         <v>43133</v>
       </c>
       <c r="E8" s="11">
-        <v>0.66666666666666663</v>
+        <v>0.6875</v>
       </c>
       <c r="F8" s="12">
         <v>43133</v>
       </c>
       <c r="G8" s="11">
-        <v>0.66666666666666663</v>
+        <v>0.6875</v>
       </c>
       <c r="H8" s="10">
         <v>0</v>
@@ -1109,12 +1195,14 @@
     </row>
     <row r="9" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="12"/>
+        <v>44</v>
+      </c>
+      <c r="C9" s="26">
+        <v>60</v>
+      </c>
       <c r="D9" s="12"/>
       <c r="E9" s="11"/>
       <c r="F9" s="12"/>
@@ -1126,12 +1214,14 @@
     </row>
     <row r="10" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="12"/>
+        <v>45</v>
+      </c>
+      <c r="C10" s="26">
+        <v>25</v>
+      </c>
       <c r="D10" s="12"/>
       <c r="E10" s="11"/>
       <c r="F10" s="12"/>
@@ -1143,12 +1233,14 @@
     </row>
     <row r="11" spans="1:11" s="6" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="12"/>
+        <v>46</v>
+      </c>
+      <c r="C11" s="26">
+        <v>60</v>
+      </c>
       <c r="D11" s="12">
         <v>43137</v>
       </c>
@@ -1164,12 +1256,14 @@
     </row>
     <row r="12" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="12"/>
+        <v>43</v>
+      </c>
+      <c r="C12" s="26">
+        <v>40</v>
+      </c>
       <c r="D12" s="12">
         <v>43137</v>
       </c>
@@ -1182,28 +1276,30 @@
       <c r="I12" s="9"/>
       <c r="J12" s="8"/>
       <c r="K12" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="12"/>
+        <v>47</v>
+      </c>
+      <c r="C13" s="26">
+        <v>10</v>
+      </c>
       <c r="D13" s="12">
         <v>43133</v>
       </c>
       <c r="E13" s="11">
-        <v>0.75</v>
+        <v>0.75694444444444453</v>
       </c>
       <c r="F13" s="12">
         <v>43133</v>
       </c>
       <c r="G13" s="11">
-        <v>0.75</v>
+        <v>0.75694444444444453</v>
       </c>
       <c r="H13" s="10">
         <v>0</v>
@@ -1214,12 +1310,14 @@
     </row>
     <row r="14" spans="1:11" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="12"/>
+        <v>47</v>
+      </c>
+      <c r="C14" s="26">
+        <v>15</v>
+      </c>
       <c r="D14" s="12">
         <v>43137</v>
       </c>
@@ -1235,12 +1333,14 @@
     </row>
     <row r="15" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="12"/>
+        <v>47</v>
+      </c>
+      <c r="C15" s="26">
+        <v>20</v>
+      </c>
       <c r="D15" s="12"/>
       <c r="E15" s="11"/>
       <c r="F15" s="12"/>
@@ -1252,10 +1352,14 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
+        <v>26</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="26">
+        <v>10</v>
+      </c>
       <c r="D16" s="12">
         <v>43136</v>
       </c>
@@ -1269,7 +1373,7 @@
         <v>0.67013888888888884</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I16" s="17"/>
       <c r="J16" s="16"/>
@@ -1277,12 +1381,14 @@
     </row>
     <row r="17" spans="1:11" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="12"/>
+        <v>47</v>
+      </c>
+      <c r="C17" s="26">
+        <v>15</v>
+      </c>
       <c r="D17" s="12">
         <v>43137</v>
       </c>
@@ -1298,12 +1404,14 @@
     </row>
     <row r="18" spans="1:11" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="12"/>
+        <v>47</v>
+      </c>
+      <c r="C18" s="26">
+        <v>15</v>
+      </c>
       <c r="D18" s="12">
         <v>43137</v>
       </c>
@@ -1319,12 +1427,14 @@
     </row>
     <row r="19" spans="1:11" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="12"/>
+        <v>43</v>
+      </c>
+      <c r="C19" s="26">
+        <v>20</v>
+      </c>
       <c r="D19" s="12">
         <v>43137</v>
       </c>
@@ -1340,12 +1450,14 @@
     </row>
     <row r="20" spans="1:11" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="12"/>
+        <v>45</v>
+      </c>
+      <c r="C20" s="26">
+        <v>20</v>
+      </c>
       <c r="D20" s="12">
         <v>43137</v>
       </c>
@@ -1361,12 +1473,14 @@
     </row>
     <row r="21" spans="1:11" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="12"/>
+        <v>46</v>
+      </c>
+      <c r="C21" s="26">
+        <v>20</v>
+      </c>
       <c r="D21" s="12">
         <v>43137</v>
       </c>
@@ -1382,12 +1496,14 @@
     </row>
     <row r="22" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="12"/>
+        <v>44</v>
+      </c>
+      <c r="C22" s="26">
+        <v>20</v>
+      </c>
       <c r="D22" s="12">
         <v>43137</v>
       </c>
@@ -1403,18 +1519,16 @@
     </row>
     <row r="23" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12">
-        <v>43137</v>
-      </c>
-      <c r="E23" s="11">
-        <v>0.875</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="26">
+        <v>20</v>
+      </c>
+      <c r="D23" s="12"/>
+      <c r="E23" s="11"/>
       <c r="F23" s="12"/>
       <c r="G23" s="11"/>
       <c r="H23" s="10"/>
@@ -1424,17 +1538,19 @@
     </row>
     <row r="24" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="12"/>
+        <v>48</v>
+      </c>
+      <c r="C24" s="26">
+        <v>20</v>
+      </c>
       <c r="D24" s="12">
         <v>43137</v>
       </c>
       <c r="E24" s="11">
-        <v>0.72916666666666663</v>
+        <v>0.875</v>
       </c>
       <c r="F24" s="12"/>
       <c r="G24" s="11"/>
@@ -1445,17 +1561,19 @@
     </row>
     <row r="25" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="12"/>
+        <v>47</v>
+      </c>
+      <c r="C25" s="26">
+        <v>25</v>
+      </c>
       <c r="D25" s="12">
         <v>43137</v>
       </c>
       <c r="E25" s="11">
-        <v>0.89583333333333337</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="F25" s="12"/>
       <c r="G25" s="11"/>
@@ -1466,14 +1584,20 @@
     </row>
     <row r="26" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="11"/>
+        <v>46</v>
+      </c>
+      <c r="C26" s="26">
+        <v>15</v>
+      </c>
+      <c r="D26" s="12">
+        <v>43137</v>
+      </c>
+      <c r="E26" s="11">
+        <v>0.89583333333333337</v>
+      </c>
       <c r="F26" s="12"/>
       <c r="G26" s="11"/>
       <c r="H26" s="10"/>
@@ -1483,18 +1607,16 @@
     </row>
     <row r="27" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="26">
         <v>0</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12">
-        <v>43137</v>
-      </c>
-      <c r="E27" s="11">
-        <v>0.91666666666666663</v>
-      </c>
+      <c r="D27" s="12"/>
+      <c r="E27" s="11"/>
       <c r="F27" s="12"/>
       <c r="G27" s="11"/>
       <c r="H27" s="10"/>
@@ -1504,17 +1626,19 @@
     </row>
     <row r="28" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="12"/>
+        <v>48</v>
+      </c>
+      <c r="C28" s="26">
+        <v>10</v>
+      </c>
       <c r="D28" s="12">
         <v>43137</v>
       </c>
       <c r="E28" s="11">
-        <v>0.93055555555555547</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="F28" s="12"/>
       <c r="G28" s="11"/>
@@ -1524,15 +1648,21 @@
       <c r="K28" s="7"/>
     </row>
     <row r="29" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
-        <v>20</v>
+      <c r="A29" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="11"/>
+        <v>49</v>
+      </c>
+      <c r="C29" s="26">
+        <v>5</v>
+      </c>
+      <c r="D29" s="12">
+        <v>43137</v>
+      </c>
+      <c r="E29" s="11">
+        <v>0.93055555555555547</v>
+      </c>
       <c r="F29" s="12"/>
       <c r="G29" s="11"/>
       <c r="H29" s="10"/>
@@ -1541,37 +1671,37 @@
       <c r="K29" s="7"/>
     </row>
     <row r="30" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12">
-        <v>43137</v>
-      </c>
-      <c r="E30" s="11">
-        <v>0.9375</v>
-      </c>
+      <c r="A30" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="26"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="11"/>
       <c r="F30" s="12"/>
       <c r="G30" s="11"/>
       <c r="H30" s="10"/>
       <c r="I30" s="9"/>
       <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
+      <c r="K30" s="7"/>
     </row>
     <row r="31" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="12"/>
+      <c r="C31" s="26">
+        <v>10</v>
+      </c>
       <c r="D31" s="12">
         <v>43137</v>
       </c>
       <c r="E31" s="11">
-        <v>0.94791666666666663</v>
+        <v>0.9375</v>
       </c>
       <c r="F31" s="12"/>
       <c r="G31" s="11"/>
@@ -1582,17 +1712,19 @@
     </row>
     <row r="32" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="12"/>
+      <c r="C32" s="26">
+        <v>15</v>
+      </c>
       <c r="D32" s="12">
-        <v>43138</v>
+        <v>43137</v>
       </c>
       <c r="E32" s="11">
-        <v>0.45833333333333331</v>
+        <v>0.94791666666666663</v>
       </c>
       <c r="F32" s="12"/>
       <c r="G32" s="11"/>
@@ -1601,42 +1733,121 @@
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
     </row>
-    <row r="33" spans="1:11" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
+    <row r="33" spans="1:11" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="26">
+        <v>20</v>
+      </c>
       <c r="D33" s="12">
-        <v>43137</v>
+        <v>43138</v>
       </c>
       <c r="E33" s="11">
-        <v>0.95833333333333337</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="F33" s="12"/>
       <c r="G33" s="11"/>
       <c r="H33" s="10"/>
       <c r="I33" s="9"/>
       <c r="J33" s="8"/>
-      <c r="K33" s="7"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K34" s="5"/>
+      <c r="K33" s="8"/>
+    </row>
+    <row r="34" spans="1:11" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="26">
+        <v>30</v>
+      </c>
+      <c r="D34" s="12">
+        <v>43137</v>
+      </c>
+      <c r="E34" s="11">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="F34" s="12"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="7"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K35" s="5"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="K36" s="5"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="28">
+        <f>C8+C12+C13+C14+C15+C16+C17+C18+C19+C25+C31+C32</f>
+        <v>215</v>
+      </c>
       <c r="K37" s="5"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="28">
+        <f>C10+C13+C15+C14+C17+C16+C18+C20+C25+C31+C32+C33+C8</f>
+        <v>220</v>
+      </c>
       <c r="K38" s="5"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="28">
+        <f>C8+C11+C13+C14+C15+C16+C17+C18+C21+C26+C31+C32</f>
+        <v>225</v>
+      </c>
       <c r="K39" s="5"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" s="28">
+        <f>C8+C9+C14+C13+C16+C15+C18+C17+C22+C29+C31+C32</f>
+        <v>215</v>
+      </c>
+      <c r="K40" s="5"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" s="28">
+        <f>C8++C13+C14+C16+C15+C17+C18+C24+C25+C29+C31+C32+C28</f>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="28">
+        <f>C34+C23+C18+C17+C16+C15+C14+C13+C8</f>
+        <v>155</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>